<commit_message>
Update bug list for M2
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
   <si>
     <t>#</t>
   </si>
@@ -82,6 +82,9 @@
     <t>P4</t>
   </si>
   <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
     <t>Projectiles from player to enemies are inconsistent, seems like only when bounding boxes are just barely overlapping</t>
   </si>
   <si>
@@ -112,6 +115,18 @@
     <t>Wait until enough entities spawn and overlap on top of each other</t>
   </si>
   <si>
+    <t>During damage lock, when the player has taken damge and will be invincible for a short ms, the projectiles pass through it. The projectile correctly doesn't apply damage but it should also disappear</t>
+  </si>
+  <si>
+    <t>Projectiles should disappear when hitting the player even if they don't take damage</t>
+  </si>
+  <si>
+    <t>Player doesn't take damage but projectile keeps going</t>
+  </si>
+  <si>
+    <t>Stand still and allow player to get hit by more than one projectile</t>
+  </si>
+  <si>
     <t>P0</t>
   </si>
   <si>
@@ -125,6 +140,45 @@
   </si>
   <si>
     <t>Move player into an enemy entity</t>
+  </si>
+  <si>
+    <t>Crashes when player dies</t>
+  </si>
+  <si>
+    <t>Game should restart without crashing</t>
+  </si>
+  <si>
+    <t>Player dies and give it time for game to try restarting</t>
+  </si>
+  <si>
+    <t>Lightning and water barrier spells have a much larger bounding box than expected</t>
+  </si>
+  <si>
+    <t>Bounding boxes should be more accurate to sprite size</t>
+  </si>
+  <si>
+    <t>The spells are colliding when we don't expect it to since bounding boxes are too large</t>
+  </si>
+  <si>
+    <t>Turn on debug mode and cast lightning / water spell</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Keys besides clicking and space bar let us continue from tutorial</t>
+  </si>
+  <si>
+    <t>Only clicking or space bar should allow us to continue from tutorial</t>
+  </si>
+  <si>
+    <t>Other keys allow us to continue from tutorial</t>
+  </si>
+  <si>
+    <t>Use other keys in the tutorial screen</t>
   </si>
 </sst>
 </file>
@@ -335,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -393,9 +447,24 @@
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
     <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -412,24 +481,6 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -735,7 +786,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="17.13"/>
     <col customWidth="1" min="2" max="6" width="27.63"/>
-    <col customWidth="1" min="7" max="7" width="94.0"/>
+    <col customWidth="1" min="7" max="7" width="89.63"/>
     <col customWidth="1" min="8" max="8" width="77.25"/>
     <col customWidth="1" min="9" max="9" width="68.0"/>
     <col customWidth="1" min="10" max="10" width="60.38"/>
@@ -852,22 +903,22 @@
         <v>22</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -878,28 +929,28 @@
         <v>45574.0</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G5" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I5" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -910,10 +961,10 @@
         <v>45576.0</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>12</v>
@@ -935,344 +986,432 @@
       </c>
     </row>
     <row r="7">
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
+      <c r="A7" s="12">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="13">
+        <v>45576.0</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="25"/>
+      <c r="A8" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="5">
+        <v>45598.0</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="30"/>
-      <c r="J9" s="31"/>
+      <c r="A9" s="12">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="13">
+        <v>45598.0</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="25"/>
+      <c r="A10" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="5">
+        <v>45598.0</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-      <c r="J11" s="31"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="24"/>
     </row>
     <row r="12">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="30"/>
     </row>
     <row r="13">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="31"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="25"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="30"/>
     </row>
     <row r="15">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="31"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="30"/>
     </row>
     <row r="17">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="31"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="24"/>
     </row>
     <row r="18">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="30"/>
     </row>
     <row r="19">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="31"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="25"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
     </row>
     <row r="21">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="31"/>
+      <c r="A21" s="19"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="30"/>
     </row>
     <row r="23">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="31"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="24"/>
     </row>
     <row r="24">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="25"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
     </row>
     <row r="25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="31"/>
+      <c r="A25" s="19"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="24"/>
     </row>
     <row r="26">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="25"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="30"/>
     </row>
     <row r="27">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="31"/>
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="22"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="24"/>
     </row>
     <row r="28">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="25"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="30"/>
     </row>
     <row r="29">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="31"/>
+      <c r="A29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="22"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="24"/>
     </row>
     <row r="30">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="25"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="30"/>
     </row>
     <row r="31">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="31"/>
+      <c r="A31" s="19"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="25"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="30"/>
     </row>
     <row r="33">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="31"/>
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="25"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="30"/>
     </row>
     <row r="35">
-      <c r="A35" s="32"/>
-      <c r="B35" s="33"/>
-      <c r="C35" s="33"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="37"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="35"/>
+      <c r="H35" s="35"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="36"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">

</xml_diff>

<commit_message>
Update bug report for M3
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
   <si>
     <t>#</t>
   </si>
@@ -179,6 +179,72 @@
   </si>
   <si>
     <t>Use other keys in the tutorial screen</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>Player animation will not reset to movement direction if an attack is triggered while walking</t>
+  </si>
+  <si>
+    <t>Should briefly change direction for the attack, and then change back to their direction of movement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stays facing the attack direction (e.g. N) while continuing to move (e.g W) </t>
+  </si>
+  <si>
+    <t>Move in one direction and attack in another</t>
+  </si>
+  <si>
+    <t>Only one shard of the ice spell applies damage</t>
+  </si>
+  <si>
+    <t>Any number of ice shards that hits an enemy should be registered to hit damage</t>
+  </si>
+  <si>
+    <t>Only one shard applies damage</t>
+  </si>
+  <si>
+    <t>Hit an enemy with more than one ice shard</t>
+  </si>
+  <si>
+    <t>Player will often automatically move after the game has been restarted</t>
+  </si>
+  <si>
+    <t>Player should be stationary at game start</t>
+  </si>
+  <si>
+    <t>Player moves in a seemingly random direction, and will not stop until that key is pressed</t>
+  </si>
+  <si>
+    <t>Hold movement keys as death timer counts down</t>
+  </si>
+  <si>
+    <t>Blinking after attack animation</t>
+  </si>
+  <si>
+    <t>Attack animation should transition smoothly back into walk/idle</t>
+  </si>
+  <si>
+    <t>There is a brief blink changing back, visually distracting</t>
+  </si>
+  <si>
+    <t>Attack as player or have enemies trigger attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ricky </t>
+  </si>
+  <si>
+    <t>Player doesn't face in proper direction when casting</t>
+  </si>
+  <si>
+    <t>Player faces close to direction of mouse when casting</t>
+  </si>
+  <si>
+    <t>Player is forced to face right when casting</t>
+  </si>
+  <si>
+    <t>Cast while not facing right</t>
   </si>
 </sst>
 </file>
@@ -215,7 +281,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border/>
     <border>
       <left style="thin">
@@ -345,13 +411,27 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF292F50"/>
       </left>
       <right style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF292F50"/>
@@ -359,13 +439,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </right>
       <top style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF292F50"/>
@@ -373,13 +453,13 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </left>
       <right style="thin">
         <color rgb="FF292F50"/>
       </right>
       <top style="thin">
-        <color rgb="FFF6F8F9"/>
+        <color rgb="FFFFFFFF"/>
       </top>
       <bottom style="thin">
         <color rgb="FF292F50"/>
@@ -389,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -447,6 +527,27 @@
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -465,40 +566,22 @@
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -559,7 +642,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J35" displayName="BUG_LIST" name="BUG_LIST" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J36" displayName="BUG_LIST" name="BUG_LIST" id="1">
   <tableColumns count="10">
     <tableColumn name="#" id="1"/>
     <tableColumn name="Reported Date" id="2"/>
@@ -1114,304 +1197,416 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="24"/>
+      <c r="A11" s="12">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="13">
+        <v>45600.0</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="18" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="25"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="30"/>
+      <c r="A12" s="19">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="5">
+        <v>45607.0</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
+      <c r="A13" s="12">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="13">
+        <v>45609.0</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="18" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="30"/>
+      <c r="A14" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="5">
+        <v>45613.0</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="24"/>
+      <c r="A15" s="12">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="13">
+        <v>45615.0</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="30"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
     </row>
     <row r="17">
-      <c r="A17" s="19"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="24"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="29"/>
-      <c r="I18" s="29"/>
-      <c r="J18" s="30"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25"/>
     </row>
     <row r="19">
-      <c r="A19" s="19"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="24"/>
+      <c r="A19" s="26"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="30"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="25"/>
     </row>
     <row r="21">
-      <c r="A21" s="19"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+      <c r="J21" s="31"/>
     </row>
     <row r="22">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="30"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="25"/>
     </row>
     <row r="23">
-      <c r="A23" s="19"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="30"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
     </row>
     <row r="25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="24"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+      <c r="J25" s="31"/>
     </row>
     <row r="26">
-      <c r="A26" s="25"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="30"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="25"/>
     </row>
     <row r="27">
-      <c r="A27" s="19"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="24"/>
+      <c r="A27" s="26"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="30"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="25"/>
     </row>
     <row r="29">
-      <c r="A29" s="19"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="24"/>
+      <c r="A29" s="26"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="31"/>
     </row>
     <row r="30">
-      <c r="A30" s="25"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="30"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="25"/>
     </row>
     <row r="31">
-      <c r="A31" s="19"/>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="22"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="24"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="31"/>
     </row>
     <row r="32">
-      <c r="A32" s="25"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="27"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="30"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="25"/>
     </row>
     <row r="33">
-      <c r="A33" s="19"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="24"/>
+      <c r="A33" s="26"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
+      <c r="J33" s="31"/>
     </row>
     <row r="34">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="30"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="24"/>
+      <c r="I34" s="24"/>
+      <c r="J34" s="25"/>
     </row>
     <row r="35">
-      <c r="A35" s="31"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="33"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="35"/>
-      <c r="H35" s="35"/>
-      <c r="I35" s="35"/>
-      <c r="J35" s="36"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="31"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="32"/>
+      <c r="B36" s="33"/>
+      <c r="C36" s="33"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="35"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="37"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
@@ -1425,10 +1620,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D35">
+    <dataValidation type="list" allowBlank="1" sqref="D2:D36">
       <formula1>"P0,P1,P2,P3,P4,P5"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="E2:E35">
+    <dataValidation type="list" allowBlank="1" sqref="E2:E36">
       <formula1>"Open,In-Progress,Resolved,Won't Fix"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Balance Adjustments + Boss Squad (#173)
* fixes + adjustments

* fix lightning multiple

* More balancing and Ricky's changes

* add boss protection detail

* add lightning damage type

* stop ice repeat damage + increase upgrade count

* Scaling health and Ricky's changes

* Missed temporary spell queue change

* Updated bug report for M4

---------

Co-authored-by: Ricky <rickyzhl@students.cs.ubc.ca>
Co-authored-by: Josh Fung <joshuagyfung@gmail.com>
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="89">
   <si>
     <t>#</t>
   </si>
@@ -82,9 +82,6 @@
     <t>P4</t>
   </si>
   <si>
-    <t>In-Progress</t>
-  </si>
-  <si>
     <t>Projectiles from player to enemies are inconsistent, seems like only when bounding boxes are just barely overlapping</t>
   </si>
   <si>
@@ -245,6 +242,42 @@
   </si>
   <si>
     <t>Cast while not facing right</t>
+  </si>
+  <si>
+    <t>Some combination of inputs (e.g. can't press E while walking) are malfunctioning</t>
+  </si>
+  <si>
+    <t>Player should be able to walk and press E to heal at the same time</t>
+  </si>
+  <si>
+    <t>Pressing E to heal doesn't work while the player is walking</t>
+  </si>
+  <si>
+    <t>Simultaneouly walk and heal using 'E' (when healing is not on cooldown)</t>
+  </si>
+  <si>
+    <t>Enemy projectiles are traveling through the player on-hit instead of being destroyed</t>
+  </si>
+  <si>
+    <t>Enemy projectile should disappearing when it collides with the player (even if player is invincible)</t>
+  </si>
+  <si>
+    <t>Enemy projectile is not destroyed on collision with player. Instead, it keeps travelling.</t>
+  </si>
+  <si>
+    <t>Allow the player to be hit with an enemy projectile</t>
+  </si>
+  <si>
+    <t>Max level ice spell hits enemies numerous times</t>
+  </si>
+  <si>
+    <t>The spell should only damage enemies ONCE</t>
+  </si>
+  <si>
+    <t>The spell damages enemies FIVE times (at most)</t>
+  </si>
+  <si>
+    <t>Attack enemies using the max level ice spell</t>
   </si>
 </sst>
 </file>
@@ -530,6 +563,24 @@
     <xf borderId="10" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
+    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+    </xf>
+    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
@@ -546,24 +597,6 @@
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -986,22 +1019,22 @@
         <v>22</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="5">
@@ -1012,28 +1045,28 @@
         <v>45574.0</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>29</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I5" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="J5" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6">
@@ -1044,7 +1077,7 @@
         <v>45576.0</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>11</v>
@@ -1056,16 +1089,16 @@
         <v>21</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="11" t="s">
         <v>36</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7">
@@ -1076,10 +1109,10 @@
         <v>45576.0</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>12</v>
@@ -1088,16 +1121,16 @@
         <v>21</v>
       </c>
       <c r="G7" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="I7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="17" t="s">
+      <c r="J7" s="18" t="s">
         <v>41</v>
-      </c>
-      <c r="J7" s="18" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8">
@@ -1111,7 +1144,7 @@
         <v>21</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" s="7" t="s">
         <v>12</v>
@@ -1120,16 +1153,16 @@
         <v>21</v>
       </c>
       <c r="G8" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J8" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="9">
@@ -1152,16 +1185,16 @@
         <v>21</v>
       </c>
       <c r="G9" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="I9" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="17" t="s">
+      <c r="J9" s="18" t="s">
         <v>48</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10">
@@ -1172,28 +1205,28 @@
         <v>45598.0</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="H10" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="J10" s="11" t="s">
         <v>54</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="11">
@@ -1204,28 +1237,28 @@
         <v>45600.0</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>12</v>
       </c>
       <c r="F11" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="H11" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="I11" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="I11" s="17" t="s">
+      <c r="J11" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="J11" s="18" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="12">
@@ -1239,7 +1272,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>12</v>
@@ -1248,16 +1281,16 @@
         <v>21</v>
       </c>
       <c r="G12" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="I12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="J12" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13">
@@ -1268,10 +1301,10 @@
         <v>45609.0</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>12</v>
@@ -1280,16 +1313,16 @@
         <v>10</v>
       </c>
       <c r="G13" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="I13" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="17" t="s">
+      <c r="J13" s="18" t="s">
         <v>67</v>
-      </c>
-      <c r="J13" s="18" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14">
@@ -1300,7 +1333,7 @@
         <v>45613.0</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>11</v>
@@ -1309,19 +1342,19 @@
         <v>12</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="I14" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="J14" s="11" t="s">
         <v>71</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -1332,7 +1365,7 @@
         <v>45615.0</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D15" s="15" t="s">
         <v>11</v>
@@ -1344,257 +1377,317 @@
         <v>10</v>
       </c>
       <c r="G15" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="I15" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="J15" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="J15" s="18" t="s">
+    </row>
+    <row r="16">
+      <c r="A16" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="5">
+        <v>45624.0</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="25"/>
+      <c r="H16" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
-      <c r="J17" s="31"/>
+      <c r="A17" s="12">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="13">
+        <v>45624.0</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
+      <c r="A18" s="4">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="5">
+        <v>45625.0</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="31"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
     </row>
     <row r="20">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="25"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21">
-      <c r="A21" s="26"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="31"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="25"/>
     </row>
     <row r="22">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="25"/>
+      <c r="A22" s="26"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
+      <c r="J22" s="31"/>
     </row>
     <row r="23">
-      <c r="A23" s="26"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="30"/>
-      <c r="J23" s="31"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="25"/>
     </row>
     <row r="24">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="25"/>
+      <c r="A24" s="26"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="30"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="30"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="30"/>
-      <c r="J25" s="31"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="25"/>
     </row>
     <row r="26">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="25"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+      <c r="J26" s="31"/>
     </row>
     <row r="27">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="30"/>
-      <c r="J27" s="31"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="25"/>
     </row>
     <row r="28">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="25"/>
+      <c r="A28" s="26"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29">
-      <c r="A29" s="26"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="31"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="25"/>
     </row>
     <row r="30">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="25"/>
+      <c r="A30" s="26"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31">
-      <c r="A31" s="26"/>
-      <c r="B31" s="27"/>
-      <c r="C31" s="27"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="30"/>
-      <c r="J31" s="31"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="25"/>
     </row>
     <row r="32">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="25"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="31"/>
     </row>
     <row r="33">
-      <c r="A33" s="26"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="28"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="30"/>
-      <c r="J33" s="31"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="25"/>
     </row>
     <row r="34">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="25"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="30"/>
+      <c r="J34" s="31"/>
     </row>
     <row r="35">
-      <c r="A35" s="26"/>
-      <c r="B35" s="27"/>
-      <c r="C35" s="27"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="31"/>
+      <c r="A35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="24"/>
+      <c r="I35" s="24"/>
+      <c r="J35" s="25"/>
     </row>
     <row r="36">
       <c r="A36" s="32"/>

</xml_diff>